<commit_message>
Added Abandoned building 1 and 2
</commit_message>
<xml_diff>
--- a/building_stats.xlsx
+++ b/building_stats.xlsx
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,11 +1183,11 @@
         <v>29</v>
       </c>
       <c r="C2" s="2">
-        <f>A2*E2*E2</f>
+        <f t="shared" ref="C2:C65" si="0">A2*E2*E2</f>
         <v>53256</v>
       </c>
       <c r="D2" s="2">
-        <f>A2*E2</f>
+        <f t="shared" ref="D2:D65" si="1">A2*E2</f>
         <v>53256</v>
       </c>
       <c r="E2">
@@ -1205,11 +1205,11 @@
         <v>30</v>
       </c>
       <c r="C3" s="2">
-        <f>A3*E3*E3</f>
+        <f t="shared" si="0"/>
         <v>50439</v>
       </c>
       <c r="D3" s="2">
-        <f>A3*E3</f>
+        <f t="shared" si="1"/>
         <v>50439</v>
       </c>
       <c r="E3">
@@ -1227,11 +1227,11 @@
         <v>12</v>
       </c>
       <c r="C4" s="2">
-        <f>A4*E4*E4</f>
+        <f t="shared" si="0"/>
         <v>33979</v>
       </c>
       <c r="D4" s="2">
-        <f>A4*E4</f>
+        <f t="shared" si="1"/>
         <v>33979</v>
       </c>
       <c r="E4">
@@ -1249,11 +1249,11 @@
         <v>7</v>
       </c>
       <c r="C5" s="2">
-        <f>A5*E5*E5</f>
+        <f t="shared" si="0"/>
         <v>28110</v>
       </c>
       <c r="D5" s="2">
-        <f>A5*E5</f>
+        <f t="shared" si="1"/>
         <v>28110</v>
       </c>
       <c r="E5">
@@ -1271,11 +1271,11 @@
         <v>11</v>
       </c>
       <c r="C6" s="2">
-        <f>A6*E6*E6</f>
+        <f t="shared" si="0"/>
         <v>21867</v>
       </c>
       <c r="D6" s="2">
-        <f>A6*E6</f>
+        <f t="shared" si="1"/>
         <v>21867</v>
       </c>
       <c r="E6">
@@ -1293,11 +1293,11 @@
         <v>6</v>
       </c>
       <c r="C7" s="2">
-        <f>A7*E7*E7</f>
+        <f t="shared" si="0"/>
         <v>20549</v>
       </c>
       <c r="D7" s="2">
-        <f>A7*E7</f>
+        <f t="shared" si="1"/>
         <v>20549</v>
       </c>
       <c r="E7">
@@ -1315,11 +1315,11 @@
         <v>8</v>
       </c>
       <c r="C8" s="2">
-        <f>A8*E8*E8</f>
+        <f t="shared" si="0"/>
         <v>20179</v>
       </c>
       <c r="D8" s="2">
-        <f>A8*E8</f>
+        <f t="shared" si="1"/>
         <v>20179</v>
       </c>
       <c r="E8">
@@ -1337,11 +1337,11 @@
         <v>9</v>
       </c>
       <c r="C9" s="2">
-        <f>A9*E9*E9</f>
+        <f t="shared" si="0"/>
         <v>14557</v>
       </c>
       <c r="D9" s="2">
-        <f>A9*E9</f>
+        <f t="shared" si="1"/>
         <v>14557</v>
       </c>
       <c r="E9">
@@ -1359,11 +1359,11 @@
         <v>220</v>
       </c>
       <c r="C10" s="2">
-        <f>A10*E10*E10</f>
+        <f t="shared" si="0"/>
         <v>12830</v>
       </c>
       <c r="D10" s="2">
-        <f>A10*E10</f>
+        <f t="shared" si="1"/>
         <v>12830</v>
       </c>
       <c r="E10">
@@ -1381,11 +1381,11 @@
         <v>10</v>
       </c>
       <c r="C11" s="2">
-        <f>A11*E11*E11</f>
+        <f t="shared" si="0"/>
         <v>11365</v>
       </c>
       <c r="D11" s="2">
-        <f>A11*E11</f>
+        <f t="shared" si="1"/>
         <v>11365</v>
       </c>
       <c r="E11">
@@ -1403,11 +1403,11 @@
         <v>13</v>
       </c>
       <c r="C12" s="2">
-        <f>A12*E12*E12</f>
+        <f t="shared" si="0"/>
         <v>9419</v>
       </c>
       <c r="D12" s="2">
-        <f>A12*E12</f>
+        <f t="shared" si="1"/>
         <v>9419</v>
       </c>
       <c r="E12">
@@ -1425,11 +1425,11 @@
         <v>147</v>
       </c>
       <c r="C13" s="2">
-        <f>A13*E13*E13</f>
+        <f t="shared" si="0"/>
         <v>16344</v>
       </c>
       <c r="D13" s="2">
-        <f>A13*E13</f>
+        <f t="shared" si="1"/>
         <v>8172</v>
       </c>
       <c r="E13">
@@ -1447,11 +1447,11 @@
         <v>145</v>
       </c>
       <c r="C14" s="2">
-        <f>A14*E14*E14</f>
+        <f t="shared" si="0"/>
         <v>16300</v>
       </c>
       <c r="D14" s="2">
-        <f>A14*E14</f>
+        <f t="shared" si="1"/>
         <v>8150</v>
       </c>
       <c r="E14">
@@ -1469,11 +1469,11 @@
         <v>146</v>
       </c>
       <c r="C15" s="2">
-        <f>A15*E15*E15</f>
+        <f t="shared" si="0"/>
         <v>16208</v>
       </c>
       <c r="D15" s="2">
-        <f>A15*E15</f>
+        <f t="shared" si="1"/>
         <v>8104</v>
       </c>
       <c r="E15">
@@ -1491,11 +1491,11 @@
         <v>144</v>
       </c>
       <c r="C16" s="2">
-        <f>A16*E16*E16</f>
+        <f t="shared" si="0"/>
         <v>16080</v>
       </c>
       <c r="D16" s="2">
-        <f>A16*E16</f>
+        <f t="shared" si="1"/>
         <v>8040</v>
       </c>
       <c r="E16">
@@ -1513,11 +1513,11 @@
         <v>120</v>
       </c>
       <c r="C17" s="2">
-        <f>A17*E17*E17</f>
+        <f t="shared" si="0"/>
         <v>6915</v>
       </c>
       <c r="D17" s="2">
-        <f>A17*E17</f>
+        <f t="shared" si="1"/>
         <v>6915</v>
       </c>
       <c r="E17">
@@ -1535,11 +1535,11 @@
         <v>67</v>
       </c>
       <c r="C18" s="2">
-        <f>A18*E18*E18</f>
+        <f t="shared" si="0"/>
         <v>6899</v>
       </c>
       <c r="D18" s="2">
-        <f>A18*E18</f>
+        <f t="shared" si="1"/>
         <v>6899</v>
       </c>
       <c r="E18">
@@ -1557,11 +1557,11 @@
         <v>121</v>
       </c>
       <c r="C19" s="2">
-        <f>A19*E19*E19</f>
+        <f t="shared" si="0"/>
         <v>6764</v>
       </c>
       <c r="D19" s="2">
-        <f>A19*E19</f>
+        <f t="shared" si="1"/>
         <v>6764</v>
       </c>
       <c r="E19">
@@ -1579,11 +1579,11 @@
         <v>68</v>
       </c>
       <c r="C20" s="2">
-        <f>A20*E20*E20</f>
+        <f t="shared" si="0"/>
         <v>6681</v>
       </c>
       <c r="D20" s="2">
-        <f>A20*E20</f>
+        <f t="shared" si="1"/>
         <v>6681</v>
       </c>
       <c r="E20">
@@ -1601,11 +1601,11 @@
         <v>123</v>
       </c>
       <c r="C21" s="2">
-        <f>A21*E21*E21</f>
+        <f t="shared" si="0"/>
         <v>6525</v>
       </c>
       <c r="D21" s="2">
-        <f>A21*E21</f>
+        <f t="shared" si="1"/>
         <v>6525</v>
       </c>
       <c r="E21">
@@ -1623,11 +1623,11 @@
         <v>134</v>
       </c>
       <c r="C22" s="2">
-        <f>A22*E22*E22</f>
+        <f t="shared" si="0"/>
         <v>6362</v>
       </c>
       <c r="D22" s="2">
-        <f>A22*E22</f>
+        <f t="shared" si="1"/>
         <v>6362</v>
       </c>
       <c r="E22">
@@ -1645,11 +1645,11 @@
         <v>133</v>
       </c>
       <c r="C23" s="2">
-        <f>A23*E23*E23</f>
+        <f t="shared" si="0"/>
         <v>6291</v>
       </c>
       <c r="D23" s="2">
-        <f>A23*E23</f>
+        <f t="shared" si="1"/>
         <v>6291</v>
       </c>
       <c r="E23">
@@ -1667,11 +1667,11 @@
         <v>135</v>
       </c>
       <c r="C24" s="2">
-        <f>A24*E24*E24</f>
+        <f t="shared" si="0"/>
         <v>6258</v>
       </c>
       <c r="D24" s="2">
-        <f>A24*E24</f>
+        <f t="shared" si="1"/>
         <v>6258</v>
       </c>
       <c r="E24">
@@ -1689,11 +1689,11 @@
         <v>122</v>
       </c>
       <c r="C25" s="2">
-        <f>A25*E25*E25</f>
+        <f t="shared" si="0"/>
         <v>6211</v>
       </c>
       <c r="D25" s="2">
-        <f>A25*E25</f>
+        <f t="shared" si="1"/>
         <v>6211</v>
       </c>
       <c r="E25">
@@ -1711,11 +1711,11 @@
         <v>132</v>
       </c>
       <c r="C26" s="2">
-        <f>A26*E26*E26</f>
+        <f t="shared" si="0"/>
         <v>6126</v>
       </c>
       <c r="D26" s="2">
-        <f>A26*E26</f>
+        <f t="shared" si="1"/>
         <v>6126</v>
       </c>
       <c r="E26">
@@ -1733,11 +1733,11 @@
         <v>117</v>
       </c>
       <c r="C27" s="2">
-        <f>A27*E27*E27</f>
+        <f t="shared" si="0"/>
         <v>6104</v>
       </c>
       <c r="D27" s="2">
-        <f>A27*E27</f>
+        <f t="shared" si="1"/>
         <v>6104</v>
       </c>
       <c r="E27">
@@ -1755,11 +1755,11 @@
         <v>116</v>
       </c>
       <c r="C28" s="2">
-        <f>A28*E28*E28</f>
+        <f t="shared" si="0"/>
         <v>6100</v>
       </c>
       <c r="D28" s="2">
-        <f>A28*E28</f>
+        <f t="shared" si="1"/>
         <v>6100</v>
       </c>
       <c r="E28">
@@ -1777,11 +1777,11 @@
         <v>118</v>
       </c>
       <c r="C29" s="2">
-        <f>A29*E29*E29</f>
+        <f t="shared" si="0"/>
         <v>6089</v>
       </c>
       <c r="D29" s="2">
-        <f>A29*E29</f>
+        <f t="shared" si="1"/>
         <v>6089</v>
       </c>
       <c r="E29">
@@ -1799,11 +1799,11 @@
         <v>119</v>
       </c>
       <c r="C30" s="2">
-        <f>A30*E30*E30</f>
+        <f t="shared" si="0"/>
         <v>6042</v>
       </c>
       <c r="D30" s="2">
-        <f>A30*E30</f>
+        <f t="shared" si="1"/>
         <v>6042</v>
       </c>
       <c r="E30">
@@ -1821,11 +1821,11 @@
         <v>210</v>
       </c>
       <c r="C31" s="2">
-        <f>A31*E31*E31</f>
+        <f t="shared" si="0"/>
         <v>14337</v>
       </c>
       <c r="D31" s="2">
-        <f>A31*E31</f>
+        <f t="shared" si="1"/>
         <v>4779</v>
       </c>
       <c r="E31">
@@ -1843,11 +1843,11 @@
         <v>74</v>
       </c>
       <c r="C32" s="2">
-        <f>A32*E32*E32</f>
+        <f t="shared" si="0"/>
         <v>4745</v>
       </c>
       <c r="D32" s="2">
-        <f>A32*E32</f>
+        <f t="shared" si="1"/>
         <v>4745</v>
       </c>
       <c r="E32">
@@ -1865,11 +1865,11 @@
         <v>73</v>
       </c>
       <c r="C33" s="2">
-        <f>A33*E33*E33</f>
+        <f t="shared" si="0"/>
         <v>4603</v>
       </c>
       <c r="D33" s="2">
-        <f>A33*E33</f>
+        <f t="shared" si="1"/>
         <v>4603</v>
       </c>
       <c r="E33">
@@ -1887,11 +1887,11 @@
         <v>254</v>
       </c>
       <c r="C34" s="1">
-        <f>A34*E34*E34</f>
+        <f t="shared" si="0"/>
         <v>15872</v>
       </c>
       <c r="D34" s="1">
-        <f>A34*E34</f>
+        <f t="shared" si="1"/>
         <v>3968</v>
       </c>
       <c r="E34">
@@ -1909,11 +1909,11 @@
         <v>127</v>
       </c>
       <c r="C35" s="2">
-        <f>A35*E35*E35</f>
+        <f t="shared" si="0"/>
         <v>3942</v>
       </c>
       <c r="D35" s="2">
-        <f>A35*E35</f>
+        <f t="shared" si="1"/>
         <v>3942</v>
       </c>
       <c r="E35">
@@ -1931,11 +1931,11 @@
         <v>128</v>
       </c>
       <c r="C36" s="2">
-        <f>A36*E36*E36</f>
+        <f t="shared" si="0"/>
         <v>3932</v>
       </c>
       <c r="D36" s="2">
-        <f>A36*E36</f>
+        <f t="shared" si="1"/>
         <v>3932</v>
       </c>
       <c r="E36">
@@ -1953,11 +1953,11 @@
         <v>129</v>
       </c>
       <c r="C37" s="2">
-        <f>A37*E37*E37</f>
+        <f t="shared" si="0"/>
         <v>3918</v>
       </c>
       <c r="D37" s="2">
-        <f>A37*E37</f>
+        <f t="shared" si="1"/>
         <v>3918</v>
       </c>
       <c r="E37">
@@ -1975,11 +1975,11 @@
         <v>130</v>
       </c>
       <c r="C38" s="2">
-        <f>A38*E38*E38</f>
+        <f t="shared" si="0"/>
         <v>3892</v>
       </c>
       <c r="D38" s="2">
-        <f>A38*E38</f>
+        <f t="shared" si="1"/>
         <v>3892</v>
       </c>
       <c r="E38">
@@ -1997,11 +1997,11 @@
         <v>43</v>
       </c>
       <c r="C39" s="2">
-        <f>A39*E39*E39</f>
+        <f t="shared" si="0"/>
         <v>3842</v>
       </c>
       <c r="D39" s="2">
-        <f>A39*E39</f>
+        <f t="shared" si="1"/>
         <v>3842</v>
       </c>
       <c r="E39">
@@ -2019,11 +2019,11 @@
         <v>126</v>
       </c>
       <c r="C40" s="2">
-        <f>A40*E40*E40</f>
+        <f t="shared" si="0"/>
         <v>3830</v>
       </c>
       <c r="D40" s="2">
-        <f>A40*E40</f>
+        <f t="shared" si="1"/>
         <v>3830</v>
       </c>
       <c r="E40">
@@ -2041,11 +2041,11 @@
         <v>124</v>
       </c>
       <c r="C41" s="2">
-        <f>A41*E41*E41</f>
+        <f t="shared" si="0"/>
         <v>3810</v>
       </c>
       <c r="D41" s="2">
-        <f>A41*E41</f>
+        <f t="shared" si="1"/>
         <v>3810</v>
       </c>
       <c r="E41">
@@ -2063,11 +2063,11 @@
         <v>131</v>
       </c>
       <c r="C42" s="2">
-        <f>A42*E42*E42</f>
+        <f t="shared" si="0"/>
         <v>3801</v>
       </c>
       <c r="D42" s="2">
-        <f>A42*E42</f>
+        <f t="shared" si="1"/>
         <v>3801</v>
       </c>
       <c r="E42">
@@ -2085,11 +2085,11 @@
         <v>125</v>
       </c>
       <c r="C43" s="2">
-        <f>A43*E43*E43</f>
+        <f t="shared" si="0"/>
         <v>3795</v>
       </c>
       <c r="D43" s="2">
-        <f>A43*E43</f>
+        <f t="shared" si="1"/>
         <v>3795</v>
       </c>
       <c r="E43">
@@ -2107,11 +2107,11 @@
         <v>154</v>
       </c>
       <c r="C44" s="2">
-        <f>A44*E44*E44</f>
+        <f t="shared" si="0"/>
         <v>7108</v>
       </c>
       <c r="D44" s="2">
-        <f>A44*E44</f>
+        <f t="shared" si="1"/>
         <v>3554</v>
       </c>
       <c r="E44">
@@ -2129,11 +2129,11 @@
         <v>153</v>
       </c>
       <c r="C45" s="2">
-        <f>A45*E45*E45</f>
+        <f t="shared" si="0"/>
         <v>7044</v>
       </c>
       <c r="D45" s="2">
-        <f>A45*E45</f>
+        <f t="shared" si="1"/>
         <v>3522</v>
       </c>
       <c r="E45">
@@ -2151,11 +2151,11 @@
         <v>155</v>
       </c>
       <c r="C46" s="2">
-        <f>A46*E46*E46</f>
+        <f t="shared" si="0"/>
         <v>7004</v>
       </c>
       <c r="D46" s="2">
-        <f>A46*E46</f>
+        <f t="shared" si="1"/>
         <v>3502</v>
       </c>
       <c r="E46">
@@ -2173,11 +2173,11 @@
         <v>156</v>
       </c>
       <c r="C47" s="2">
-        <f>A47*E47*E47</f>
+        <f t="shared" si="0"/>
         <v>6968</v>
       </c>
       <c r="D47" s="2">
-        <f>A47*E47</f>
+        <f t="shared" si="1"/>
         <v>3484</v>
       </c>
       <c r="E47">
@@ -2195,11 +2195,11 @@
         <v>37</v>
       </c>
       <c r="C48" s="2">
-        <f>A48*E48*E48</f>
+        <f t="shared" si="0"/>
         <v>3468</v>
       </c>
       <c r="D48" s="2">
-        <f>A48*E48</f>
+        <f t="shared" si="1"/>
         <v>3468</v>
       </c>
       <c r="E48">
@@ -2217,11 +2217,11 @@
         <v>35</v>
       </c>
       <c r="C49" s="2">
-        <f>A49*E49*E49</f>
+        <f t="shared" si="0"/>
         <v>3464</v>
       </c>
       <c r="D49" s="2">
-        <f>A49*E49</f>
+        <f t="shared" si="1"/>
         <v>3464</v>
       </c>
       <c r="E49">
@@ -2239,11 +2239,11 @@
         <v>38</v>
       </c>
       <c r="C50" s="2">
-        <f>A50*E50*E50</f>
+        <f t="shared" si="0"/>
         <v>3300</v>
       </c>
       <c r="D50" s="2">
-        <f>A50*E50</f>
+        <f t="shared" si="1"/>
         <v>3300</v>
       </c>
       <c r="E50">
@@ -2261,11 +2261,11 @@
         <v>36</v>
       </c>
       <c r="C51" s="2">
-        <f>A51*E51*E51</f>
+        <f t="shared" si="0"/>
         <v>3284</v>
       </c>
       <c r="D51" s="2">
-        <f>A51*E51</f>
+        <f t="shared" si="1"/>
         <v>3284</v>
       </c>
       <c r="E51">
@@ -2283,11 +2283,11 @@
         <v>157</v>
       </c>
       <c r="C52" s="2">
-        <f>A52*E52*E52</f>
+        <f t="shared" si="0"/>
         <v>6464</v>
       </c>
       <c r="D52" s="2">
-        <f>A52*E52</f>
+        <f t="shared" si="1"/>
         <v>3232</v>
       </c>
       <c r="E52">
@@ -2305,11 +2305,11 @@
         <v>163</v>
       </c>
       <c r="C53" s="2">
-        <f>A53*E53*E53</f>
+        <f t="shared" si="0"/>
         <v>5468</v>
       </c>
       <c r="D53" s="2">
-        <f>A53*E53</f>
+        <f t="shared" si="1"/>
         <v>2734</v>
       </c>
       <c r="E53">
@@ -2327,11 +2327,11 @@
         <v>164</v>
       </c>
       <c r="C54" s="2">
-        <f>A54*E54*E54</f>
+        <f t="shared" si="0"/>
         <v>5464</v>
       </c>
       <c r="D54" s="2">
-        <f>A54*E54</f>
+        <f t="shared" si="1"/>
         <v>2732</v>
       </c>
       <c r="E54">
@@ -2345,15 +2345,15 @@
       <c r="A55">
         <v>2717</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="2">
         <v>139</v>
       </c>
-      <c r="C55" s="1">
-        <f>A55*E55*E55</f>
+      <c r="C55" s="2">
+        <f t="shared" si="0"/>
         <v>2717</v>
       </c>
-      <c r="D55" s="1">
-        <f>A55*E55</f>
+      <c r="D55" s="2">
+        <f t="shared" si="1"/>
         <v>2717</v>
       </c>
       <c r="E55">
@@ -2367,15 +2367,15 @@
       <c r="A56">
         <v>2710</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="2">
         <v>138</v>
       </c>
-      <c r="C56" s="1">
-        <f>A56*E56*E56</f>
+      <c r="C56" s="2">
+        <f t="shared" si="0"/>
         <v>2710</v>
       </c>
-      <c r="D56" s="1">
-        <f>A56*E56</f>
+      <c r="D56" s="2">
+        <f t="shared" si="1"/>
         <v>2710</v>
       </c>
       <c r="E56">
@@ -2393,11 +2393,11 @@
         <v>165</v>
       </c>
       <c r="C57" s="2">
-        <f>A57*E57*E57</f>
+        <f t="shared" si="0"/>
         <v>5256</v>
       </c>
       <c r="D57" s="2">
-        <f>A57*E57</f>
+        <f t="shared" si="1"/>
         <v>2628</v>
       </c>
       <c r="E57">
@@ -2415,11 +2415,11 @@
         <v>227</v>
       </c>
       <c r="C58" s="2">
-        <f>A58*E58*E58</f>
+        <f t="shared" si="0"/>
         <v>2621</v>
       </c>
       <c r="D58" s="2">
-        <f>A58*E58</f>
+        <f t="shared" si="1"/>
         <v>2621</v>
       </c>
       <c r="E58">
@@ -2437,11 +2437,11 @@
         <v>162</v>
       </c>
       <c r="C59" s="2">
-        <f>A59*E59*E59</f>
+        <f t="shared" si="0"/>
         <v>5236</v>
       </c>
       <c r="D59" s="2">
-        <f>A59*E59</f>
+        <f t="shared" si="1"/>
         <v>2618</v>
       </c>
       <c r="E59">
@@ -2459,11 +2459,11 @@
         <v>40</v>
       </c>
       <c r="C60" s="2">
-        <f>A60*E60*E60</f>
+        <f t="shared" si="0"/>
         <v>2535</v>
       </c>
       <c r="D60" s="2">
-        <f>A60*E60</f>
+        <f t="shared" si="1"/>
         <v>2535</v>
       </c>
       <c r="E60">
@@ -2481,11 +2481,11 @@
         <v>214</v>
       </c>
       <c r="C61" s="2">
-        <f>A61*E61*E61</f>
+        <f t="shared" si="0"/>
         <v>7596</v>
       </c>
       <c r="D61" s="2">
-        <f>A61*E61</f>
+        <f t="shared" si="1"/>
         <v>2532</v>
       </c>
       <c r="E61">
@@ -2503,11 +2503,11 @@
         <v>41</v>
       </c>
       <c r="C62" s="2">
-        <f>A62*E62*E62</f>
+        <f t="shared" si="0"/>
         <v>2497</v>
       </c>
       <c r="D62" s="2">
-        <f>A62*E62</f>
+        <f t="shared" si="1"/>
         <v>2497</v>
       </c>
       <c r="E62">
@@ -2525,11 +2525,11 @@
         <v>42</v>
       </c>
       <c r="C63" s="2">
-        <f>A63*E63*E63</f>
+        <f t="shared" si="0"/>
         <v>2490</v>
       </c>
       <c r="D63" s="2">
-        <f>A63*E63</f>
+        <f t="shared" si="1"/>
         <v>2490</v>
       </c>
       <c r="E63">
@@ -2547,11 +2547,11 @@
         <v>39</v>
       </c>
       <c r="C64" s="2">
-        <f>A64*E64*E64</f>
+        <f t="shared" si="0"/>
         <v>2479</v>
       </c>
       <c r="D64" s="2">
-        <f>A64*E64</f>
+        <f t="shared" si="1"/>
         <v>2479</v>
       </c>
       <c r="E64">
@@ -2569,11 +2569,11 @@
         <v>213</v>
       </c>
       <c r="C65" s="1">
-        <f>A65*E65*E65</f>
+        <f t="shared" si="0"/>
         <v>7389</v>
       </c>
       <c r="D65" s="1">
-        <f>A65*E65</f>
+        <f t="shared" si="1"/>
         <v>2463</v>
       </c>
       <c r="E65">
@@ -2591,11 +2591,11 @@
         <v>141</v>
       </c>
       <c r="C66" s="1">
-        <f>A66*E66*E66</f>
+        <f t="shared" ref="C66:C129" si="2">A66*E66*E66</f>
         <v>4660</v>
       </c>
       <c r="D66" s="1">
-        <f>A66*E66</f>
+        <f t="shared" ref="D66:D129" si="3">A66*E66</f>
         <v>2330</v>
       </c>
       <c r="E66">
@@ -2613,11 +2613,11 @@
         <v>143</v>
       </c>
       <c r="C67" s="2">
-        <f>A67*E67*E67</f>
+        <f t="shared" si="2"/>
         <v>4616</v>
       </c>
       <c r="D67" s="2">
-        <f>A67*E67</f>
+        <f t="shared" si="3"/>
         <v>2308</v>
       </c>
       <c r="E67">
@@ -2635,11 +2635,11 @@
         <v>140</v>
       </c>
       <c r="C68" s="2">
-        <f>A68*E68*E68</f>
+        <f t="shared" si="2"/>
         <v>4612</v>
       </c>
       <c r="D68" s="2">
-        <f>A68*E68</f>
+        <f t="shared" si="3"/>
         <v>2306</v>
       </c>
       <c r="E68">
@@ -2657,11 +2657,11 @@
         <v>113</v>
       </c>
       <c r="C69" s="2">
-        <f>A69*E69*E69</f>
+        <f t="shared" si="2"/>
         <v>2242</v>
       </c>
       <c r="D69" s="2">
-        <f>A69*E69</f>
+        <f t="shared" si="3"/>
         <v>2242</v>
       </c>
       <c r="E69">
@@ -2679,11 +2679,11 @@
         <v>142</v>
       </c>
       <c r="C70" s="1">
-        <f>A70*E70*E70</f>
+        <f t="shared" si="2"/>
         <v>4480</v>
       </c>
       <c r="D70" s="1">
-        <f>A70*E70</f>
+        <f t="shared" si="3"/>
         <v>2240</v>
       </c>
       <c r="E70">
@@ -2701,11 +2701,11 @@
         <v>115</v>
       </c>
       <c r="C71" s="2">
-        <f>A71*E71*E71</f>
+        <f t="shared" si="2"/>
         <v>2231</v>
       </c>
       <c r="D71" s="2">
-        <f>A71*E71</f>
+        <f t="shared" si="3"/>
         <v>2231</v>
       </c>
       <c r="E71">
@@ -2723,11 +2723,11 @@
         <v>114</v>
       </c>
       <c r="C72" s="2">
-        <f>A72*E72*E72</f>
+        <f t="shared" si="2"/>
         <v>2185</v>
       </c>
       <c r="D72" s="2">
-        <f>A72*E72</f>
+        <f t="shared" si="3"/>
         <v>2185</v>
       </c>
       <c r="E72">
@@ -2745,11 +2745,11 @@
         <v>112</v>
       </c>
       <c r="C73" s="2">
-        <f>A73*E73*E73</f>
+        <f t="shared" si="2"/>
         <v>2177</v>
       </c>
       <c r="D73" s="2">
-        <f>A73*E73</f>
+        <f t="shared" si="3"/>
         <v>2177</v>
       </c>
       <c r="E73">
@@ -2767,11 +2767,11 @@
         <v>45</v>
       </c>
       <c r="C74" s="2">
-        <f>A74*E74*E74</f>
+        <f t="shared" si="2"/>
         <v>2143</v>
       </c>
       <c r="D74" s="2">
-        <f>A74*E74</f>
+        <f t="shared" si="3"/>
         <v>2143</v>
       </c>
       <c r="E74">
@@ -2789,11 +2789,11 @@
         <v>44</v>
       </c>
       <c r="C75" s="2">
-        <f>A75*E75*E75</f>
+        <f t="shared" si="2"/>
         <v>2119</v>
       </c>
       <c r="D75" s="2">
-        <f>A75*E75</f>
+        <f t="shared" si="3"/>
         <v>2119</v>
       </c>
       <c r="E75">
@@ -2811,11 +2811,11 @@
         <v>199</v>
       </c>
       <c r="C76" s="1">
-        <f>A76*E76*E76</f>
+        <f t="shared" si="2"/>
         <v>1942</v>
       </c>
       <c r="D76" s="1">
-        <f>A76*E76</f>
+        <f t="shared" si="3"/>
         <v>1942</v>
       </c>
       <c r="E76">
@@ -2833,11 +2833,11 @@
         <v>236</v>
       </c>
       <c r="C77" s="1">
-        <f>A77*E77*E77</f>
+        <f t="shared" si="2"/>
         <v>3808</v>
       </c>
       <c r="D77" s="1">
-        <f>A77*E77</f>
+        <f t="shared" si="3"/>
         <v>1904</v>
       </c>
       <c r="E77">
@@ -2855,11 +2855,11 @@
         <v>198</v>
       </c>
       <c r="C78" s="1">
-        <f>A78*E78*E78</f>
+        <f t="shared" si="2"/>
         <v>1821</v>
       </c>
       <c r="D78" s="1">
-        <f>A78*E78</f>
+        <f t="shared" si="3"/>
         <v>1821</v>
       </c>
       <c r="E78">
@@ -2877,11 +2877,11 @@
         <v>211</v>
       </c>
       <c r="C79" s="2">
-        <f>A79*E79*E79</f>
+        <f t="shared" si="2"/>
         <v>5274</v>
       </c>
       <c r="D79" s="2">
-        <f>A79*E79</f>
+        <f t="shared" si="3"/>
         <v>1758</v>
       </c>
       <c r="E79">
@@ -2899,11 +2899,11 @@
         <v>233</v>
       </c>
       <c r="C80" s="1">
-        <f>A80*E80*E80</f>
+        <f t="shared" si="2"/>
         <v>1685</v>
       </c>
       <c r="D80" s="1">
-        <f>A80*E80</f>
+        <f t="shared" si="3"/>
         <v>1685</v>
       </c>
       <c r="E80">
@@ -2921,11 +2921,11 @@
         <v>221</v>
       </c>
       <c r="C81" s="2">
-        <f>A81*E81*E81</f>
+        <f t="shared" si="2"/>
         <v>1671</v>
       </c>
       <c r="D81" s="2">
-        <f>A81*E81</f>
+        <f t="shared" si="3"/>
         <v>1671</v>
       </c>
       <c r="E81">
@@ -2943,11 +2943,11 @@
         <v>247</v>
       </c>
       <c r="C82" s="2">
-        <f>A82*E82*E82</f>
+        <f t="shared" si="2"/>
         <v>3316</v>
       </c>
       <c r="D82" s="2">
-        <f>A82*E82</f>
+        <f t="shared" si="3"/>
         <v>1658</v>
       </c>
       <c r="E82">
@@ -2965,11 +2965,11 @@
         <v>32</v>
       </c>
       <c r="C83" s="2">
-        <f>A83*E83*E83</f>
+        <f t="shared" si="2"/>
         <v>1534</v>
       </c>
       <c r="D83" s="2">
-        <f>A83*E83</f>
+        <f t="shared" si="3"/>
         <v>1534</v>
       </c>
       <c r="E83">
@@ -2987,11 +2987,11 @@
         <v>209</v>
       </c>
       <c r="C84" s="2">
-        <f>A84*E84*E84</f>
+        <f t="shared" si="2"/>
         <v>4563</v>
       </c>
       <c r="D84" s="2">
-        <f>A84*E84</f>
+        <f t="shared" si="3"/>
         <v>1521</v>
       </c>
       <c r="E84">
@@ -3009,11 +3009,11 @@
         <v>15</v>
       </c>
       <c r="C85" s="2">
-        <f>A85*E85*E85</f>
+        <f t="shared" si="2"/>
         <v>1404</v>
       </c>
       <c r="D85" s="2">
-        <f>A85*E85</f>
+        <f t="shared" si="3"/>
         <v>1404</v>
       </c>
       <c r="E85">
@@ -3031,11 +3031,11 @@
         <v>14</v>
       </c>
       <c r="C86" s="2">
-        <f>A86*E86*E86</f>
+        <f t="shared" si="2"/>
         <v>1368</v>
       </c>
       <c r="D86" s="2">
-        <f>A86*E86</f>
+        <f t="shared" si="3"/>
         <v>1368</v>
       </c>
       <c r="E86">
@@ -3053,11 +3053,11 @@
         <v>31</v>
       </c>
       <c r="C87" s="2">
-        <f>A87*E87*E87</f>
+        <f t="shared" si="2"/>
         <v>1360</v>
       </c>
       <c r="D87" s="2">
-        <f>A87*E87</f>
+        <f t="shared" si="3"/>
         <v>1360</v>
       </c>
       <c r="E87">
@@ -3075,11 +3075,11 @@
         <v>223</v>
       </c>
       <c r="C88" s="2">
-        <f>A88*E88*E88</f>
+        <f t="shared" si="2"/>
         <v>1311</v>
       </c>
       <c r="D88" s="2">
-        <f>A88*E88</f>
+        <f t="shared" si="3"/>
         <v>1311</v>
       </c>
       <c r="E88">
@@ -3097,11 +3097,11 @@
         <v>248</v>
       </c>
       <c r="C89" s="1">
-        <f>A89*E89*E89</f>
+        <f t="shared" si="2"/>
         <v>3879</v>
       </c>
       <c r="D89" s="1">
-        <f>A89*E89</f>
+        <f t="shared" si="3"/>
         <v>1293</v>
       </c>
       <c r="E89">
@@ -3119,11 +3119,11 @@
         <v>33</v>
       </c>
       <c r="C90" s="2">
-        <f>A90*E90*E90</f>
+        <f t="shared" si="2"/>
         <v>1173</v>
       </c>
       <c r="D90" s="2">
-        <f>A90*E90</f>
+        <f t="shared" si="3"/>
         <v>1173</v>
       </c>
       <c r="E90">
@@ -3141,11 +3141,11 @@
         <v>92</v>
       </c>
       <c r="C91" s="1">
-        <f>A91*E91*E91</f>
+        <f t="shared" si="2"/>
         <v>1107</v>
       </c>
       <c r="D91" s="1">
-        <f>A91*E91</f>
+        <f t="shared" si="3"/>
         <v>1107</v>
       </c>
       <c r="E91">
@@ -3163,11 +3163,11 @@
         <v>245</v>
       </c>
       <c r="C92" s="1">
-        <f>A92*E92*E92</f>
+        <f t="shared" si="2"/>
         <v>2208</v>
       </c>
       <c r="D92" s="1">
-        <f>A92*E92</f>
+        <f t="shared" si="3"/>
         <v>1104</v>
       </c>
       <c r="E92">
@@ -3185,11 +3185,11 @@
         <v>34</v>
       </c>
       <c r="C93" s="2">
-        <f>A93*E93*E93</f>
+        <f t="shared" si="2"/>
         <v>1090</v>
       </c>
       <c r="D93" s="2">
-        <f>A93*E93</f>
+        <f t="shared" si="3"/>
         <v>1090</v>
       </c>
       <c r="E93">
@@ -3207,11 +3207,11 @@
         <v>17</v>
       </c>
       <c r="C94" s="2">
-        <f>A94*E94*E94</f>
+        <f t="shared" si="2"/>
         <v>983</v>
       </c>
       <c r="D94" s="2">
-        <f>A94*E94</f>
+        <f t="shared" si="3"/>
         <v>983</v>
       </c>
       <c r="E94">
@@ -3229,11 +3229,11 @@
         <v>217</v>
       </c>
       <c r="C95" s="1">
-        <f>A95*E95*E95</f>
+        <f t="shared" si="2"/>
         <v>3712</v>
       </c>
       <c r="D95" s="1">
-        <f>A95*E95</f>
+        <f t="shared" si="3"/>
         <v>928</v>
       </c>
       <c r="E95">
@@ -3251,11 +3251,11 @@
         <v>16</v>
       </c>
       <c r="C96" s="2">
-        <f>A96*E96*E96</f>
+        <f t="shared" si="2"/>
         <v>863</v>
       </c>
       <c r="D96" s="2">
-        <f>A96*E96</f>
+        <f t="shared" si="3"/>
         <v>863</v>
       </c>
       <c r="E96">
@@ -3273,11 +3273,11 @@
         <v>87</v>
       </c>
       <c r="C97" s="1">
-        <f>A97*E97*E97</f>
+        <f t="shared" si="2"/>
         <v>858</v>
       </c>
       <c r="D97" s="1">
-        <f>A97*E97</f>
+        <f t="shared" si="3"/>
         <v>858</v>
       </c>
       <c r="E97">
@@ -3295,11 +3295,11 @@
         <v>192</v>
       </c>
       <c r="C98" s="2">
-        <f>A98*E98*E98</f>
+        <f t="shared" si="2"/>
         <v>2556</v>
       </c>
       <c r="D98" s="2">
-        <f>A98*E98</f>
+        <f t="shared" si="3"/>
         <v>852</v>
       </c>
       <c r="E98">
@@ -3317,11 +3317,11 @@
         <v>193</v>
       </c>
       <c r="C99" s="1">
-        <f>A99*E99*E99</f>
+        <f t="shared" si="2"/>
         <v>2502</v>
       </c>
       <c r="D99" s="1">
-        <f>A99*E99</f>
+        <f t="shared" si="3"/>
         <v>834</v>
       </c>
       <c r="E99">
@@ -3339,11 +3339,11 @@
         <v>212</v>
       </c>
       <c r="C100" s="1">
-        <f>A100*E100*E100</f>
+        <f t="shared" si="2"/>
         <v>2457</v>
       </c>
       <c r="D100" s="1">
-        <f>A100*E100</f>
+        <f t="shared" si="3"/>
         <v>819</v>
       </c>
       <c r="E100">
@@ -3361,11 +3361,11 @@
         <v>190</v>
       </c>
       <c r="C101" s="1">
-        <f>A101*E101*E101</f>
+        <f t="shared" si="2"/>
         <v>2430</v>
       </c>
       <c r="D101" s="1">
-        <f>A101*E101</f>
+        <f t="shared" si="3"/>
         <v>810</v>
       </c>
       <c r="E101">
@@ -3383,11 +3383,11 @@
         <v>191</v>
       </c>
       <c r="C102" s="2">
-        <f>A102*E102*E102</f>
+        <f t="shared" si="2"/>
         <v>2322</v>
       </c>
       <c r="D102" s="2">
-        <f>A102*E102</f>
+        <f t="shared" si="3"/>
         <v>774</v>
       </c>
       <c r="E102">
@@ -3405,11 +3405,11 @@
         <v>188</v>
       </c>
       <c r="C103" s="1">
-        <f>A103*E103*E103</f>
+        <f t="shared" si="2"/>
         <v>2250</v>
       </c>
       <c r="D103" s="1">
-        <f>A103*E103</f>
+        <f t="shared" si="3"/>
         <v>750</v>
       </c>
       <c r="E103">
@@ -3427,11 +3427,11 @@
         <v>18</v>
       </c>
       <c r="C104" s="2">
-        <f>A104*E104*E104</f>
+        <f t="shared" si="2"/>
         <v>726</v>
       </c>
       <c r="D104" s="2">
-        <f>A104*E104</f>
+        <f t="shared" si="3"/>
         <v>726</v>
       </c>
       <c r="E104">
@@ -3449,11 +3449,11 @@
         <v>189</v>
       </c>
       <c r="C105" s="2">
-        <f>A105*E105*E105</f>
+        <f t="shared" si="2"/>
         <v>2169</v>
       </c>
       <c r="D105" s="2">
-        <f>A105*E105</f>
+        <f t="shared" si="3"/>
         <v>723</v>
       </c>
       <c r="E105">
@@ -3471,11 +3471,11 @@
         <v>169</v>
       </c>
       <c r="C106" s="1">
-        <f>A106*E106*E106</f>
+        <f t="shared" si="2"/>
         <v>1416</v>
       </c>
       <c r="D106" s="1">
-        <f>A106*E106</f>
+        <f t="shared" si="3"/>
         <v>708</v>
       </c>
       <c r="E106">
@@ -3493,11 +3493,11 @@
         <v>168</v>
       </c>
       <c r="C107" s="1">
-        <f>A107*E107*E107</f>
+        <f t="shared" si="2"/>
         <v>1368</v>
       </c>
       <c r="D107" s="1">
-        <f>A107*E107</f>
+        <f t="shared" si="3"/>
         <v>684</v>
       </c>
       <c r="E107">
@@ -3515,11 +3515,11 @@
         <v>228</v>
       </c>
       <c r="C108" s="1">
-        <f>A108*E108*E108</f>
+        <f t="shared" si="2"/>
         <v>658</v>
       </c>
       <c r="D108" s="1">
-        <f>A108*E108</f>
+        <f t="shared" si="3"/>
         <v>658</v>
       </c>
       <c r="E108">
@@ -3537,11 +3537,11 @@
         <v>229</v>
       </c>
       <c r="C109" s="1">
-        <f>A109*E109*E109</f>
+        <f t="shared" si="2"/>
         <v>651</v>
       </c>
       <c r="D109" s="1">
-        <f>A109*E109</f>
+        <f t="shared" si="3"/>
         <v>651</v>
       </c>
       <c r="E109">
@@ -3559,11 +3559,11 @@
         <v>235</v>
       </c>
       <c r="C110" s="1">
-        <f>A110*E110*E110</f>
+        <f t="shared" si="2"/>
         <v>1296</v>
       </c>
       <c r="D110" s="1">
-        <f>A110*E110</f>
+        <f t="shared" si="3"/>
         <v>648</v>
       </c>
       <c r="E110">
@@ -3581,11 +3581,11 @@
         <v>215</v>
       </c>
       <c r="C111" s="1">
-        <f>A111*E111*E111</f>
+        <f t="shared" si="2"/>
         <v>2528</v>
       </c>
       <c r="D111" s="1">
-        <f>A111*E111</f>
+        <f t="shared" si="3"/>
         <v>632</v>
       </c>
       <c r="E111">
@@ -3603,11 +3603,11 @@
         <v>19</v>
       </c>
       <c r="C112" s="2">
-        <f>A112*E112*E112</f>
+        <f t="shared" si="2"/>
         <v>623</v>
       </c>
       <c r="D112" s="2">
-        <f>A112*E112</f>
+        <f t="shared" si="3"/>
         <v>623</v>
       </c>
       <c r="E112">
@@ -3625,11 +3625,11 @@
         <v>76</v>
       </c>
       <c r="C113" s="1">
-        <f>A113*E113*E113</f>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="D113" s="1">
-        <f>A113*E113</f>
+        <f t="shared" si="3"/>
         <v>616</v>
       </c>
       <c r="E113">
@@ -3647,11 +3647,11 @@
         <v>200</v>
       </c>
       <c r="C114" s="1">
-        <f>A114*E114*E114</f>
+        <f t="shared" si="2"/>
         <v>611</v>
       </c>
       <c r="D114" s="1">
-        <f>A114*E114</f>
+        <f t="shared" si="3"/>
         <v>611</v>
       </c>
       <c r="E114">
@@ -3669,11 +3669,11 @@
         <v>240</v>
       </c>
       <c r="C115" s="1">
-        <f>A115*E115*E115</f>
+        <f t="shared" si="2"/>
         <v>1196</v>
       </c>
       <c r="D115" s="1">
-        <f>A115*E115</f>
+        <f t="shared" si="3"/>
         <v>598</v>
       </c>
       <c r="E115">
@@ -3691,11 +3691,11 @@
         <v>242</v>
       </c>
       <c r="C116" s="1">
-        <f>A116*E116*E116</f>
+        <f t="shared" si="2"/>
         <v>1128</v>
       </c>
       <c r="D116" s="1">
-        <f>A116*E116</f>
+        <f t="shared" si="3"/>
         <v>564</v>
       </c>
       <c r="E116">
@@ -3713,11 +3713,11 @@
         <v>246</v>
       </c>
       <c r="C117" s="1">
-        <f>A117*E117*E117</f>
+        <f t="shared" si="2"/>
         <v>1088</v>
       </c>
       <c r="D117" s="1">
-        <f>A117*E117</f>
+        <f t="shared" si="3"/>
         <v>544</v>
       </c>
       <c r="E117">
@@ -3735,11 +3735,11 @@
         <v>75</v>
       </c>
       <c r="C118" s="1">
-        <f>A118*E118*E118</f>
+        <f t="shared" si="2"/>
         <v>524</v>
       </c>
       <c r="D118" s="1">
-        <f>A118*E118</f>
+        <f t="shared" si="3"/>
         <v>524</v>
       </c>
       <c r="E118">
@@ -3757,11 +3757,11 @@
         <v>218</v>
       </c>
       <c r="C119" s="1">
-        <f>A119*E119*E119</f>
+        <f t="shared" si="2"/>
         <v>1872</v>
       </c>
       <c r="D119" s="1">
-        <f>A119*E119</f>
+        <f t="shared" si="3"/>
         <v>468</v>
       </c>
       <c r="E119">
@@ -3779,11 +3779,11 @@
         <v>237</v>
       </c>
       <c r="C120" s="1">
-        <f>A120*E120*E120</f>
+        <f t="shared" si="2"/>
         <v>936</v>
       </c>
       <c r="D120" s="1">
-        <f>A120*E120</f>
+        <f t="shared" si="3"/>
         <v>468</v>
       </c>
       <c r="E120">
@@ -3801,11 +3801,11 @@
         <v>244</v>
       </c>
       <c r="C121" s="1">
-        <f>A121*E121*E121</f>
+        <f t="shared" si="2"/>
         <v>892</v>
       </c>
       <c r="D121" s="1">
-        <f>A121*E121</f>
+        <f t="shared" si="3"/>
         <v>446</v>
       </c>
       <c r="E121">
@@ -3823,11 +3823,11 @@
         <v>238</v>
       </c>
       <c r="C122" s="1">
-        <f>A122*E122*E122</f>
+        <f t="shared" si="2"/>
         <v>880</v>
       </c>
       <c r="D122" s="1">
-        <f>A122*E122</f>
+        <f t="shared" si="3"/>
         <v>440</v>
       </c>
       <c r="E122">
@@ -3845,11 +3845,11 @@
         <v>170</v>
       </c>
       <c r="C123" s="1">
-        <f>A123*E123*E123</f>
+        <f t="shared" si="2"/>
         <v>872</v>
       </c>
       <c r="D123" s="1">
-        <f>A123*E123</f>
+        <f t="shared" si="3"/>
         <v>436</v>
       </c>
       <c r="E123">
@@ -3867,11 +3867,11 @@
         <v>171</v>
       </c>
       <c r="C124" s="1">
-        <f>A124*E124*E124</f>
+        <f t="shared" si="2"/>
         <v>820</v>
       </c>
       <c r="D124" s="1">
-        <f>A124*E124</f>
+        <f t="shared" si="3"/>
         <v>410</v>
       </c>
       <c r="E124">
@@ -3889,11 +3889,11 @@
         <v>50</v>
       </c>
       <c r="C125" s="2">
-        <f>A125*E125*E125</f>
+        <f t="shared" si="2"/>
         <v>402</v>
       </c>
       <c r="D125" s="2">
-        <f>A125*E125</f>
+        <f t="shared" si="3"/>
         <v>402</v>
       </c>
       <c r="E125">
@@ -3911,11 +3911,11 @@
         <v>52</v>
       </c>
       <c r="C126" s="2">
-        <f>A126*E126*E126</f>
+        <f t="shared" si="2"/>
         <v>399</v>
       </c>
       <c r="D126" s="2">
-        <f>A126*E126</f>
+        <f t="shared" si="3"/>
         <v>399</v>
       </c>
       <c r="E126">
@@ -3933,11 +3933,11 @@
         <v>152</v>
       </c>
       <c r="C127" s="1">
-        <f>A127*E127*E127</f>
+        <f t="shared" si="2"/>
         <v>784</v>
       </c>
       <c r="D127" s="1">
-        <f>A127*E127</f>
+        <f t="shared" si="3"/>
         <v>392</v>
       </c>
       <c r="E127">
@@ -3955,11 +3955,11 @@
         <v>175</v>
       </c>
       <c r="C128" s="1">
-        <f>A128*E128*E128</f>
+        <f t="shared" si="2"/>
         <v>1071</v>
       </c>
       <c r="D128" s="1">
-        <f>A128*E128</f>
+        <f t="shared" si="3"/>
         <v>357</v>
       </c>
       <c r="E128">
@@ -3977,11 +3977,11 @@
         <v>81</v>
       </c>
       <c r="C129" s="2">
-        <f>A129*E129*E129</f>
+        <f t="shared" si="2"/>
         <v>352</v>
       </c>
       <c r="D129" s="2">
-        <f>A129*E129</f>
+        <f t="shared" si="3"/>
         <v>352</v>
       </c>
       <c r="E129">
@@ -3999,11 +3999,11 @@
         <v>82</v>
       </c>
       <c r="C130" s="2">
-        <f>A130*E130*E130</f>
+        <f t="shared" ref="C130:C193" si="4">A130*E130*E130</f>
         <v>352</v>
       </c>
       <c r="D130" s="2">
-        <f>A130*E130</f>
+        <f t="shared" ref="D130:D193" si="5">A130*E130</f>
         <v>352</v>
       </c>
       <c r="E130">
@@ -4021,11 +4021,11 @@
         <v>83</v>
       </c>
       <c r="C131" s="2">
-        <f>A131*E131*E131</f>
+        <f t="shared" si="4"/>
         <v>352</v>
       </c>
       <c r="D131" s="2">
-        <f>A131*E131</f>
+        <f t="shared" si="5"/>
         <v>352</v>
       </c>
       <c r="E131">
@@ -4043,11 +4043,11 @@
         <v>84</v>
       </c>
       <c r="C132" s="2">
-        <f>A132*E132*E132</f>
+        <f t="shared" si="4"/>
         <v>352</v>
       </c>
       <c r="D132" s="2">
-        <f>A132*E132</f>
+        <f t="shared" si="5"/>
         <v>352</v>
       </c>
       <c r="E132">
@@ -4065,11 +4065,11 @@
         <v>85</v>
       </c>
       <c r="C133" s="2">
-        <f>A133*E133*E133</f>
+        <f t="shared" si="4"/>
         <v>352</v>
       </c>
       <c r="D133" s="2">
-        <f>A133*E133</f>
+        <f t="shared" si="5"/>
         <v>352</v>
       </c>
       <c r="E133">
@@ -4087,11 +4087,11 @@
         <v>173</v>
       </c>
       <c r="C134" s="1">
-        <f>A134*E134*E134</f>
+        <f t="shared" si="4"/>
         <v>696</v>
       </c>
       <c r="D134" s="1">
-        <f>A134*E134</f>
+        <f t="shared" si="5"/>
         <v>348</v>
       </c>
       <c r="E134">
@@ -4109,11 +4109,11 @@
         <v>251</v>
       </c>
       <c r="C135" s="1">
-        <f>A135*E135*E135</f>
+        <f t="shared" si="4"/>
         <v>1376</v>
       </c>
       <c r="D135" s="1">
-        <f>A135*E135</f>
+        <f t="shared" si="5"/>
         <v>344</v>
       </c>
       <c r="E135">
@@ -4131,11 +4131,11 @@
         <v>150</v>
       </c>
       <c r="C136" s="1">
-        <f>A136*E136*E136</f>
+        <f t="shared" si="4"/>
         <v>688</v>
       </c>
       <c r="D136" s="1">
-        <f>A136*E136</f>
+        <f t="shared" si="5"/>
         <v>344</v>
       </c>
       <c r="E136">
@@ -4153,11 +4153,11 @@
         <v>151</v>
       </c>
       <c r="C137" s="1">
-        <f>A137*E137*E137</f>
+        <f t="shared" si="4"/>
         <v>684</v>
       </c>
       <c r="D137" s="1">
-        <f>A137*E137</f>
+        <f t="shared" si="5"/>
         <v>342</v>
       </c>
       <c r="E137">
@@ -4175,11 +4175,11 @@
         <v>51</v>
       </c>
       <c r="C138" s="2">
-        <f>A138*E138*E138</f>
+        <f t="shared" si="4"/>
         <v>341</v>
       </c>
       <c r="D138" s="2">
-        <f>A138*E138</f>
+        <f t="shared" si="5"/>
         <v>341</v>
       </c>
       <c r="E138">
@@ -4197,11 +4197,11 @@
         <v>224</v>
       </c>
       <c r="C139" s="1">
-        <f>A139*E139*E139</f>
+        <f t="shared" si="4"/>
         <v>338</v>
       </c>
       <c r="D139" s="1">
-        <f>A139*E139</f>
+        <f t="shared" si="5"/>
         <v>338</v>
       </c>
       <c r="E139">
@@ -4219,11 +4219,11 @@
         <v>53</v>
       </c>
       <c r="C140" s="2">
-        <f>A140*E140*E140</f>
+        <f t="shared" si="4"/>
         <v>333</v>
       </c>
       <c r="D140" s="2">
-        <f>A140*E140</f>
+        <f t="shared" si="5"/>
         <v>333</v>
       </c>
       <c r="E140">
@@ -4241,11 +4241,11 @@
         <v>80</v>
       </c>
       <c r="C141" s="1">
-        <f>A141*E141*E141</f>
+        <f t="shared" si="4"/>
         <v>329</v>
       </c>
       <c r="D141" s="1">
-        <f>A141*E141</f>
+        <f t="shared" si="5"/>
         <v>329</v>
       </c>
       <c r="E141">
@@ -4263,11 +4263,11 @@
         <v>176</v>
       </c>
       <c r="C142" s="1">
-        <f>A142*E142*E142</f>
+        <f t="shared" si="4"/>
         <v>981</v>
       </c>
       <c r="D142" s="1">
-        <f>A142*E142</f>
+        <f t="shared" si="5"/>
         <v>327</v>
       </c>
       <c r="E142">
@@ -4285,11 +4285,11 @@
         <v>206</v>
       </c>
       <c r="C143" s="1">
-        <f>A143*E143*E143</f>
+        <f t="shared" si="4"/>
         <v>1296</v>
       </c>
       <c r="D143" s="1">
-        <f>A143*E143</f>
+        <f t="shared" si="5"/>
         <v>324</v>
       </c>
       <c r="E143">
@@ -4307,11 +4307,11 @@
         <v>149</v>
       </c>
       <c r="C144" s="1">
-        <f>A144*E144*E144</f>
+        <f t="shared" si="4"/>
         <v>644</v>
       </c>
       <c r="D144" s="1">
-        <f>A144*E144</f>
+        <f t="shared" si="5"/>
         <v>322</v>
       </c>
       <c r="E144">
@@ -4329,11 +4329,11 @@
         <v>79</v>
       </c>
       <c r="C145" s="1">
-        <f>A145*E145*E145</f>
+        <f t="shared" si="4"/>
         <v>317</v>
       </c>
       <c r="D145" s="1">
-        <f>A145*E145</f>
+        <f t="shared" si="5"/>
         <v>317</v>
       </c>
       <c r="E145">
@@ -4351,11 +4351,11 @@
         <v>148</v>
       </c>
       <c r="C146" s="1">
-        <f>A146*E146*E146</f>
+        <f t="shared" si="4"/>
         <v>628</v>
       </c>
       <c r="D146" s="1">
-        <f>A146*E146</f>
+        <f t="shared" si="5"/>
         <v>314</v>
       </c>
       <c r="E146">
@@ -4373,11 +4373,11 @@
         <v>172</v>
       </c>
       <c r="C147" s="1">
-        <f>A147*E147*E147</f>
+        <f t="shared" si="4"/>
         <v>628</v>
       </c>
       <c r="D147" s="1">
-        <f>A147*E147</f>
+        <f t="shared" si="5"/>
         <v>314</v>
       </c>
       <c r="E147">
@@ -4395,11 +4395,11 @@
         <v>177</v>
       </c>
       <c r="C148" s="1">
-        <f>A148*E148*E148</f>
+        <f t="shared" si="4"/>
         <v>936</v>
       </c>
       <c r="D148" s="1">
-        <f>A148*E148</f>
+        <f t="shared" si="5"/>
         <v>312</v>
       </c>
       <c r="E148">
@@ -4417,11 +4417,11 @@
         <v>93</v>
       </c>
       <c r="C149" s="1">
-        <f>A149*E149*E149</f>
+        <f t="shared" si="4"/>
         <v>310</v>
       </c>
       <c r="D149" s="1">
-        <f>A149*E149</f>
+        <f t="shared" si="5"/>
         <v>310</v>
       </c>
       <c r="E149">
@@ -4439,11 +4439,11 @@
         <v>230</v>
       </c>
       <c r="C150" s="1">
-        <f>A150*E150*E150</f>
+        <f t="shared" si="4"/>
         <v>305</v>
       </c>
       <c r="D150" s="1">
-        <f>A150*E150</f>
+        <f t="shared" si="5"/>
         <v>305</v>
       </c>
       <c r="E150">
@@ -4461,11 +4461,11 @@
         <v>94</v>
       </c>
       <c r="C151" s="1">
-        <f>A151*E151*E151</f>
+        <f t="shared" si="4"/>
         <v>292</v>
       </c>
       <c r="D151" s="1">
-        <f>A151*E151</f>
+        <f t="shared" si="5"/>
         <v>292</v>
       </c>
       <c r="E151">
@@ -4483,11 +4483,11 @@
         <v>95</v>
       </c>
       <c r="C152" s="1">
-        <f>A152*E152*E152</f>
+        <f t="shared" si="4"/>
         <v>291</v>
       </c>
       <c r="D152" s="1">
-        <f>A152*E152</f>
+        <f t="shared" si="5"/>
         <v>291</v>
       </c>
       <c r="E152">
@@ -4505,11 +4505,11 @@
         <v>174</v>
       </c>
       <c r="C153" s="1">
-        <f>A153*E153*E153</f>
+        <f t="shared" si="4"/>
         <v>864</v>
       </c>
       <c r="D153" s="1">
-        <f>A153*E153</f>
+        <f t="shared" si="5"/>
         <v>288</v>
       </c>
       <c r="E153">
@@ -4527,11 +4527,11 @@
         <v>104</v>
       </c>
       <c r="C154" s="1">
-        <f>A154*E154*E154</f>
+        <f t="shared" si="4"/>
         <v>572</v>
       </c>
       <c r="D154" s="1">
-        <f>A154*E154</f>
+        <f t="shared" si="5"/>
         <v>286</v>
       </c>
       <c r="E154">
@@ -4549,11 +4549,11 @@
         <v>69</v>
       </c>
       <c r="C155" s="2">
-        <f>A155*E155*E155</f>
+        <f t="shared" si="4"/>
         <v>284</v>
       </c>
       <c r="D155" s="2">
-        <f>A155*E155</f>
+        <f t="shared" si="5"/>
         <v>284</v>
       </c>
       <c r="E155">
@@ -4571,11 +4571,11 @@
         <v>70</v>
       </c>
       <c r="C156" s="2">
-        <f>A156*E156*E156</f>
+        <f t="shared" si="4"/>
         <v>278</v>
       </c>
       <c r="D156" s="2">
-        <f>A156*E156</f>
+        <f t="shared" si="5"/>
         <v>278</v>
       </c>
       <c r="E156">
@@ -4593,11 +4593,11 @@
         <v>96</v>
       </c>
       <c r="C157" s="1">
-        <f>A157*E157*E157</f>
+        <f t="shared" si="4"/>
         <v>276</v>
       </c>
       <c r="D157" s="1">
-        <f>A157*E157</f>
+        <f t="shared" si="5"/>
         <v>276</v>
       </c>
       <c r="E157">
@@ -4615,11 +4615,11 @@
         <v>102</v>
       </c>
       <c r="C158" s="1">
-        <f>A158*E158*E158</f>
+        <f t="shared" si="4"/>
         <v>548</v>
       </c>
       <c r="D158" s="1">
-        <f>A158*E158</f>
+        <f t="shared" si="5"/>
         <v>274</v>
       </c>
       <c r="E158">
@@ -4637,11 +4637,11 @@
         <v>167</v>
       </c>
       <c r="C159" s="1">
-        <f>A159*E159*E159</f>
+        <f t="shared" si="4"/>
         <v>540</v>
       </c>
       <c r="D159" s="1">
-        <f>A159*E159</f>
+        <f t="shared" si="5"/>
         <v>270</v>
       </c>
       <c r="E159">
@@ -4659,11 +4659,11 @@
         <v>166</v>
       </c>
       <c r="C160" s="1">
-        <f>A160*E160*E160</f>
+        <f t="shared" si="4"/>
         <v>496</v>
       </c>
       <c r="D160" s="1">
-        <f>A160*E160</f>
+        <f t="shared" si="5"/>
         <v>248</v>
       </c>
       <c r="E160">
@@ -4681,11 +4681,11 @@
         <v>103</v>
       </c>
       <c r="C161" s="1">
-        <f>A161*E161*E161</f>
+        <f t="shared" si="4"/>
         <v>484</v>
       </c>
       <c r="D161" s="1">
-        <f>A161*E161</f>
+        <f t="shared" si="5"/>
         <v>242</v>
       </c>
       <c r="E161">
@@ -4703,11 +4703,11 @@
         <v>101</v>
       </c>
       <c r="C162" s="1">
-        <f>A162*E162*E162</f>
+        <f t="shared" si="4"/>
         <v>476</v>
       </c>
       <c r="D162" s="1">
-        <f>A162*E162</f>
+        <f t="shared" si="5"/>
         <v>238</v>
       </c>
       <c r="E162">
@@ -4725,11 +4725,11 @@
         <v>250</v>
       </c>
       <c r="C163" s="1">
-        <f>A163*E163*E163</f>
+        <f t="shared" si="4"/>
         <v>711</v>
       </c>
       <c r="D163" s="1">
-        <f>A163*E163</f>
+        <f t="shared" si="5"/>
         <v>237</v>
       </c>
       <c r="E163">
@@ -4747,11 +4747,11 @@
         <v>182</v>
       </c>
       <c r="C164" s="1">
-        <f>A164*E164*E164</f>
+        <f t="shared" si="4"/>
         <v>702</v>
       </c>
       <c r="D164" s="1">
-        <f>A164*E164</f>
+        <f t="shared" si="5"/>
         <v>234</v>
       </c>
       <c r="E164">
@@ -4769,11 +4769,11 @@
         <v>186</v>
       </c>
       <c r="C165" s="1">
-        <f>A165*E165*E165</f>
+        <f t="shared" si="4"/>
         <v>693</v>
       </c>
       <c r="D165" s="1">
-        <f>A165*E165</f>
+        <f t="shared" si="5"/>
         <v>231</v>
       </c>
       <c r="E165">
@@ -4791,11 +4791,11 @@
         <v>178</v>
       </c>
       <c r="C166" s="1">
-        <f>A166*E166*E166</f>
+        <f t="shared" si="4"/>
         <v>684</v>
       </c>
       <c r="D166" s="1">
-        <f>A166*E166</f>
+        <f t="shared" si="5"/>
         <v>228</v>
       </c>
       <c r="E166">
@@ -4813,11 +4813,11 @@
         <v>185</v>
       </c>
       <c r="C167" s="1">
-        <f>A167*E167*E167</f>
+        <f t="shared" si="4"/>
         <v>684</v>
       </c>
       <c r="D167" s="1">
-        <f>A167*E167</f>
+        <f t="shared" si="5"/>
         <v>228</v>
       </c>
       <c r="E167">
@@ -4835,11 +4835,11 @@
         <v>20</v>
       </c>
       <c r="C168" s="2">
-        <f>A168*E168*E168</f>
+        <f t="shared" si="4"/>
         <v>228</v>
       </c>
       <c r="D168" s="2">
-        <f>A168*E168</f>
+        <f t="shared" si="5"/>
         <v>228</v>
       </c>
       <c r="E168">
@@ -4857,11 +4857,11 @@
         <v>28</v>
       </c>
       <c r="C169" s="2">
-        <f>A169*E169*E169</f>
+        <f t="shared" si="4"/>
         <v>228</v>
       </c>
       <c r="D169" s="2">
-        <f>A169*E169</f>
+        <f t="shared" si="5"/>
         <v>228</v>
       </c>
       <c r="E169">
@@ -4879,11 +4879,11 @@
         <v>22</v>
       </c>
       <c r="C170" s="2">
-        <f>A170*E170*E170</f>
+        <f t="shared" si="4"/>
         <v>226</v>
       </c>
       <c r="D170" s="2">
-        <f>A170*E170</f>
+        <f t="shared" si="5"/>
         <v>226</v>
       </c>
       <c r="E170">
@@ -4901,11 +4901,11 @@
         <v>183</v>
       </c>
       <c r="C171" s="1">
-        <f>A171*E171*E171</f>
+        <f t="shared" si="4"/>
         <v>675</v>
       </c>
       <c r="D171" s="1">
-        <f>A171*E171</f>
+        <f t="shared" si="5"/>
         <v>225</v>
       </c>
       <c r="E171">
@@ -4923,11 +4923,11 @@
         <v>187</v>
       </c>
       <c r="C172" s="2">
-        <f>A172*E172*E172</f>
+        <f t="shared" si="4"/>
         <v>675</v>
       </c>
       <c r="D172" s="2">
-        <f>A172*E172</f>
+        <f t="shared" si="5"/>
         <v>225</v>
       </c>
       <c r="E172">
@@ -4945,11 +4945,11 @@
         <v>71</v>
       </c>
       <c r="C173" s="2">
-        <f>A173*E173*E173</f>
+        <f t="shared" si="4"/>
         <v>222</v>
       </c>
       <c r="D173" s="2">
-        <f>A173*E173</f>
+        <f t="shared" si="5"/>
         <v>222</v>
       </c>
       <c r="E173">
@@ -4967,11 +4967,11 @@
         <v>208</v>
       </c>
       <c r="C174" s="1">
-        <f>A174*E174*E174</f>
+        <f t="shared" si="4"/>
         <v>657</v>
       </c>
       <c r="D174" s="1">
-        <f>A174*E174</f>
+        <f t="shared" si="5"/>
         <v>219</v>
       </c>
       <c r="E174">
@@ -4989,11 +4989,11 @@
         <v>72</v>
       </c>
       <c r="C175" s="2">
-        <f>A175*E175*E175</f>
+        <f t="shared" si="4"/>
         <v>207</v>
       </c>
       <c r="D175" s="2">
-        <f>A175*E175</f>
+        <f t="shared" si="5"/>
         <v>207</v>
       </c>
       <c r="E175">
@@ -5011,11 +5011,11 @@
         <v>158</v>
       </c>
       <c r="C176" s="1">
-        <f>A176*E176*E176</f>
+        <f t="shared" si="4"/>
         <v>412</v>
       </c>
       <c r="D176" s="1">
-        <f>A176*E176</f>
+        <f t="shared" si="5"/>
         <v>206</v>
       </c>
       <c r="E176">
@@ -5033,11 +5033,11 @@
         <v>23</v>
       </c>
       <c r="C177" s="2">
-        <f>A177*E177*E177</f>
+        <f t="shared" si="4"/>
         <v>198</v>
       </c>
       <c r="D177" s="2">
-        <f>A177*E177</f>
+        <f t="shared" si="5"/>
         <v>198</v>
       </c>
       <c r="E177">
@@ -5055,11 +5055,11 @@
         <v>234</v>
       </c>
       <c r="C178" s="1">
-        <f>A178*E178*E178</f>
+        <f t="shared" si="4"/>
         <v>198</v>
       </c>
       <c r="D178" s="1">
-        <f>A178*E178</f>
+        <f t="shared" si="5"/>
         <v>198</v>
       </c>
       <c r="E178">
@@ -5077,11 +5077,11 @@
         <v>180</v>
       </c>
       <c r="C179" s="1">
-        <f>A179*E179*E179</f>
+        <f t="shared" si="4"/>
         <v>585</v>
       </c>
       <c r="D179" s="1">
-        <f>A179*E179</f>
+        <f t="shared" si="5"/>
         <v>195</v>
       </c>
       <c r="E179">
@@ -5099,11 +5099,11 @@
         <v>181</v>
       </c>
       <c r="C180" s="1">
-        <f>A180*E180*E180</f>
+        <f t="shared" si="4"/>
         <v>585</v>
       </c>
       <c r="D180" s="1">
-        <f>A180*E180</f>
+        <f t="shared" si="5"/>
         <v>195</v>
       </c>
       <c r="E180">
@@ -5121,11 +5121,11 @@
         <v>21</v>
       </c>
       <c r="C181" s="2">
-        <f>A181*E181*E181</f>
+        <f t="shared" si="4"/>
         <v>190</v>
       </c>
       <c r="D181" s="2">
-        <f>A181*E181</f>
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
       <c r="E181">
@@ -5143,11 +5143,11 @@
         <v>225</v>
       </c>
       <c r="C182" s="1">
-        <f>A182*E182*E182</f>
+        <f t="shared" si="4"/>
         <v>184</v>
       </c>
       <c r="D182" s="1">
-        <f>A182*E182</f>
+        <f t="shared" si="5"/>
         <v>184</v>
       </c>
       <c r="E182">
@@ -5165,11 +5165,11 @@
         <v>161</v>
       </c>
       <c r="C183" s="1">
-        <f>A183*E183*E183</f>
+        <f t="shared" si="4"/>
         <v>364</v>
       </c>
       <c r="D183" s="1">
-        <f>A183*E183</f>
+        <f t="shared" si="5"/>
         <v>182</v>
       </c>
       <c r="E183">
@@ -5187,11 +5187,11 @@
         <v>179</v>
       </c>
       <c r="C184" s="1">
-        <f>A184*E184*E184</f>
+        <f t="shared" si="4"/>
         <v>540</v>
       </c>
       <c r="D184" s="1">
-        <f>A184*E184</f>
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
       <c r="E184">
@@ -5209,11 +5209,11 @@
         <v>255</v>
       </c>
       <c r="C185" s="1">
-        <f>A185*E185*E185</f>
+        <f t="shared" si="4"/>
         <v>688</v>
       </c>
       <c r="D185" s="1">
-        <f>A185*E185</f>
+        <f t="shared" si="5"/>
         <v>172</v>
       </c>
       <c r="E185">
@@ -5231,11 +5231,11 @@
         <v>184</v>
       </c>
       <c r="C186" s="1">
-        <f>A186*E186*E186</f>
+        <f t="shared" si="4"/>
         <v>513</v>
       </c>
       <c r="D186" s="1">
-        <f>A186*E186</f>
+        <f t="shared" si="5"/>
         <v>171</v>
       </c>
       <c r="E186">
@@ -5253,11 +5253,11 @@
         <v>216</v>
       </c>
       <c r="C187" s="1">
-        <f>A187*E187*E187</f>
+        <f t="shared" si="4"/>
         <v>672</v>
       </c>
       <c r="D187" s="1">
-        <f>A187*E187</f>
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
       <c r="E187">
@@ -5275,11 +5275,11 @@
         <v>4</v>
       </c>
       <c r="C188" s="1">
-        <f>A188*E188*E188</f>
+        <f t="shared" si="4"/>
         <v>166</v>
       </c>
       <c r="D188" s="1">
-        <f>A188*E188</f>
+        <f t="shared" si="5"/>
         <v>166</v>
       </c>
       <c r="E188">
@@ -5297,11 +5297,11 @@
         <v>252</v>
       </c>
       <c r="C189" s="1">
-        <f>A189*E189*E189</f>
+        <f t="shared" si="4"/>
         <v>640</v>
       </c>
       <c r="D189" s="1">
-        <f>A189*E189</f>
+        <f t="shared" si="5"/>
         <v>160</v>
       </c>
       <c r="E189">
@@ -5319,11 +5319,11 @@
         <v>1</v>
       </c>
       <c r="C190" s="1">
-        <f>A190*E190*E190</f>
+        <f t="shared" si="4"/>
         <v>158</v>
       </c>
       <c r="D190" s="1">
-        <f>A190*E190</f>
+        <f t="shared" si="5"/>
         <v>158</v>
       </c>
       <c r="E190">
@@ -5341,11 +5341,11 @@
         <v>25</v>
       </c>
       <c r="C191" s="2">
-        <f>A191*E191*E191</f>
+        <f t="shared" si="4"/>
         <v>157</v>
       </c>
       <c r="D191" s="2">
-        <f>A191*E191</f>
+        <f t="shared" si="5"/>
         <v>157</v>
       </c>
       <c r="E191">
@@ -5363,11 +5363,11 @@
         <v>90</v>
       </c>
       <c r="C192" s="1">
-        <f>A192*E192*E192</f>
+        <f t="shared" si="4"/>
         <v>155</v>
       </c>
       <c r="D192" s="1">
-        <f>A192*E192</f>
+        <f t="shared" si="5"/>
         <v>155</v>
       </c>
       <c r="E192">
@@ -5385,11 +5385,11 @@
         <v>243</v>
       </c>
       <c r="C193" s="1">
-        <f>A193*E193*E193</f>
+        <f t="shared" si="4"/>
         <v>296</v>
       </c>
       <c r="D193" s="1">
-        <f>A193*E193</f>
+        <f t="shared" si="5"/>
         <v>148</v>
       </c>
       <c r="E193">
@@ -5407,11 +5407,11 @@
         <v>160</v>
       </c>
       <c r="C194" s="1">
-        <f>A194*E194*E194</f>
+        <f t="shared" ref="C194:C257" si="6">A194*E194*E194</f>
         <v>292</v>
       </c>
       <c r="D194" s="1">
-        <f>A194*E194</f>
+        <f t="shared" ref="D194:D257" si="7">A194*E194</f>
         <v>146</v>
       </c>
       <c r="E194">
@@ -5429,11 +5429,11 @@
         <v>105</v>
       </c>
       <c r="C195" s="2">
-        <f>A195*E195*E195</f>
+        <f t="shared" si="6"/>
         <v>276</v>
       </c>
       <c r="D195" s="2">
-        <f>A195*E195</f>
+        <f t="shared" si="7"/>
         <v>138</v>
       </c>
       <c r="E195">
@@ -5451,11 +5451,11 @@
         <v>159</v>
       </c>
       <c r="C196" s="1">
-        <f>A196*E196*E196</f>
+        <f t="shared" si="6"/>
         <v>272</v>
       </c>
       <c r="D196" s="1">
-        <f>A196*E196</f>
+        <f t="shared" si="7"/>
         <v>136</v>
       </c>
       <c r="E196">
@@ -5473,11 +5473,11 @@
         <v>27</v>
       </c>
       <c r="C197" s="2">
-        <f>A197*E197*E197</f>
+        <f t="shared" si="6"/>
         <v>130</v>
       </c>
       <c r="D197" s="2">
-        <f>A197*E197</f>
+        <f t="shared" si="7"/>
         <v>130</v>
       </c>
       <c r="E197">
@@ -5495,11 +5495,11 @@
         <v>205</v>
       </c>
       <c r="C198" s="1">
-        <f>A198*E198*E198</f>
+        <f t="shared" si="6"/>
         <v>512</v>
       </c>
       <c r="D198" s="1">
-        <f>A198*E198</f>
+        <f t="shared" si="7"/>
         <v>128</v>
       </c>
       <c r="E198">
@@ -5517,11 +5517,11 @@
         <v>253</v>
       </c>
       <c r="C199" s="1">
-        <f>A199*E199*E199</f>
+        <f t="shared" si="6"/>
         <v>496</v>
       </c>
       <c r="D199" s="1">
-        <f>A199*E199</f>
+        <f t="shared" si="7"/>
         <v>124</v>
       </c>
       <c r="E199">
@@ -5539,11 +5539,11 @@
         <v>194</v>
       </c>
       <c r="C200" s="1">
-        <f>A200*E200*E200</f>
+        <f t="shared" si="6"/>
         <v>369</v>
       </c>
       <c r="D200" s="1">
-        <f>A200*E200</f>
+        <f t="shared" si="7"/>
         <v>123</v>
       </c>
       <c r="E200">
@@ -5561,11 +5561,11 @@
         <v>26</v>
       </c>
       <c r="C201" s="2">
-        <f>A201*E201*E201</f>
+        <f t="shared" si="6"/>
         <v>123</v>
       </c>
       <c r="D201" s="2">
-        <f>A201*E201</f>
+        <f t="shared" si="7"/>
         <v>123</v>
       </c>
       <c r="E201">
@@ -5583,11 +5583,11 @@
         <v>24</v>
       </c>
       <c r="C202" s="2">
-        <f>A202*E202*E202</f>
+        <f t="shared" si="6"/>
         <v>122</v>
       </c>
       <c r="D202" s="2">
-        <f>A202*E202</f>
+        <f t="shared" si="7"/>
         <v>122</v>
       </c>
       <c r="E202">
@@ -5605,11 +5605,11 @@
         <v>86</v>
       </c>
       <c r="C203" s="1">
-        <f>A203*E203*E203</f>
+        <f t="shared" si="6"/>
         <v>119</v>
       </c>
       <c r="D203" s="1">
-        <f>A203*E203</f>
+        <f t="shared" si="7"/>
         <v>119</v>
       </c>
       <c r="E203">
@@ -5627,11 +5627,11 @@
         <v>88</v>
       </c>
       <c r="C204" s="1">
-        <f>A204*E204*E204</f>
+        <f t="shared" si="6"/>
         <v>117</v>
       </c>
       <c r="D204" s="1">
-        <f>A204*E204</f>
+        <f t="shared" si="7"/>
         <v>117</v>
       </c>
       <c r="E204">
@@ -5649,11 +5649,11 @@
         <v>207</v>
       </c>
       <c r="C205" s="1">
-        <f>A205*E205*E205</f>
+        <f t="shared" si="6"/>
         <v>464</v>
       </c>
       <c r="D205" s="1">
-        <f>A205*E205</f>
+        <f t="shared" si="7"/>
         <v>116</v>
       </c>
       <c r="E205">
@@ -5671,11 +5671,11 @@
         <v>3</v>
       </c>
       <c r="C206" s="1">
-        <f>A206*E206*E206</f>
+        <f t="shared" si="6"/>
         <v>105</v>
       </c>
       <c r="D206" s="1">
-        <f>A206*E206</f>
+        <f t="shared" si="7"/>
         <v>105</v>
       </c>
       <c r="E206">
@@ -5693,11 +5693,11 @@
         <v>203</v>
       </c>
       <c r="C207" s="1">
-        <f>A207*E207*E207</f>
+        <f t="shared" si="6"/>
         <v>416</v>
       </c>
       <c r="D207" s="1">
-        <f>A207*E207</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
       <c r="E207">
@@ -5715,11 +5715,11 @@
         <v>48</v>
       </c>
       <c r="C208" s="2">
-        <f>A208*E208*E208</f>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="D208" s="2">
-        <f>A208*E208</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="E208">
@@ -5737,11 +5737,11 @@
         <v>91</v>
       </c>
       <c r="C209" s="1">
-        <f>A209*E209*E209</f>
+        <f t="shared" si="6"/>
         <v>94</v>
       </c>
       <c r="D209" s="1">
-        <f>A209*E209</f>
+        <f t="shared" si="7"/>
         <v>94</v>
       </c>
       <c r="E209">
@@ -5759,11 +5759,11 @@
         <v>232</v>
       </c>
       <c r="C210" s="1">
-        <f>A210*E210*E210</f>
+        <f t="shared" si="6"/>
         <v>93</v>
       </c>
       <c r="D210" s="1">
-        <f>A210*E210</f>
+        <f t="shared" si="7"/>
         <v>93</v>
       </c>
       <c r="E210">
@@ -5781,11 +5781,11 @@
         <v>2</v>
       </c>
       <c r="C211" s="1">
-        <f>A211*E211*E211</f>
+        <f t="shared" si="6"/>
         <v>89</v>
       </c>
       <c r="D211" s="1">
-        <f>A211*E211</f>
+        <f t="shared" si="7"/>
         <v>89</v>
       </c>
       <c r="E211">
@@ -5803,11 +5803,11 @@
         <v>195</v>
       </c>
       <c r="C212" s="1">
-        <f>A212*E212*E212</f>
+        <f t="shared" si="6"/>
         <v>252</v>
       </c>
       <c r="D212" s="1">
-        <f>A212*E212</f>
+        <f t="shared" si="7"/>
         <v>84</v>
       </c>
       <c r="E212">
@@ -5825,11 +5825,11 @@
         <v>98</v>
       </c>
       <c r="C213" s="2">
-        <f>A213*E213*E213</f>
+        <f t="shared" si="6"/>
         <v>156</v>
       </c>
       <c r="D213" s="2">
-        <f>A213*E213</f>
+        <f t="shared" si="7"/>
         <v>78</v>
       </c>
       <c r="E213">
@@ -5847,11 +5847,11 @@
         <v>97</v>
       </c>
       <c r="C214" s="2">
-        <f>A214*E214*E214</f>
+        <f t="shared" si="6"/>
         <v>152</v>
       </c>
       <c r="D214" s="2">
-        <f>A214*E214</f>
+        <f t="shared" si="7"/>
         <v>76</v>
       </c>
       <c r="E214">
@@ -5869,11 +5869,11 @@
         <v>196</v>
       </c>
       <c r="C215" s="1">
-        <f>A215*E215*E215</f>
+        <f t="shared" si="6"/>
         <v>216</v>
       </c>
       <c r="D215" s="1">
-        <f>A215*E215</f>
+        <f t="shared" si="7"/>
         <v>72</v>
       </c>
       <c r="E215">
@@ -5891,11 +5891,11 @@
         <v>49</v>
       </c>
       <c r="C216" s="2">
-        <f>A216*E216*E216</f>
+        <f t="shared" si="6"/>
         <v>69</v>
       </c>
       <c r="D216" s="2">
-        <f>A216*E216</f>
+        <f t="shared" si="7"/>
         <v>69</v>
       </c>
       <c r="E216">
@@ -5913,11 +5913,11 @@
         <v>204</v>
       </c>
       <c r="C217" s="1">
-        <f>A217*E217*E217</f>
+        <f t="shared" si="6"/>
         <v>272</v>
       </c>
       <c r="D217" s="1">
-        <f>A217*E217</f>
+        <f t="shared" si="7"/>
         <v>68</v>
       </c>
       <c r="E217">
@@ -5935,11 +5935,11 @@
         <v>197</v>
       </c>
       <c r="C218" s="1">
-        <f>A218*E218*E218</f>
+        <f t="shared" si="6"/>
         <v>198</v>
       </c>
       <c r="D218" s="1">
-        <f>A218*E218</f>
+        <f t="shared" si="7"/>
         <v>66</v>
       </c>
       <c r="E218">
@@ -5957,11 +5957,11 @@
         <v>219</v>
       </c>
       <c r="C219" s="1">
-        <f>A219*E219*E219</f>
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
       <c r="D219" s="1">
-        <f>A219*E219</f>
+        <f t="shared" si="7"/>
         <v>66</v>
       </c>
       <c r="E219">
@@ -5979,11 +5979,11 @@
         <v>222</v>
       </c>
       <c r="C220" s="1">
-        <f>A220*E220*E220</f>
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
       <c r="D220" s="1">
-        <f>A220*E220</f>
+        <f t="shared" si="7"/>
         <v>66</v>
       </c>
       <c r="E220">
@@ -6001,11 +6001,11 @@
         <v>231</v>
       </c>
       <c r="C221" s="1">
-        <f>A221*E221*E221</f>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="D221" s="1">
-        <f>A221*E221</f>
+        <f t="shared" si="7"/>
         <v>64</v>
       </c>
       <c r="E221">
@@ -6023,11 +6023,11 @@
         <v>99</v>
       </c>
       <c r="C222" s="2">
-        <f>A222*E222*E222</f>
+        <f t="shared" si="6"/>
         <v>124</v>
       </c>
       <c r="D222" s="2">
-        <f>A222*E222</f>
+        <f t="shared" si="7"/>
         <v>62</v>
       </c>
       <c r="E222">
@@ -6045,11 +6045,11 @@
         <v>226</v>
       </c>
       <c r="C223" s="1">
-        <f>A223*E223*E223</f>
+        <f t="shared" si="6"/>
         <v>61</v>
       </c>
       <c r="D223" s="1">
-        <f>A223*E223</f>
+        <f t="shared" si="7"/>
         <v>61</v>
       </c>
       <c r="E223">
@@ -6067,11 +6067,11 @@
         <v>239</v>
       </c>
       <c r="C224" s="1">
-        <f>A224*E224*E224</f>
+        <f t="shared" si="6"/>
         <v>108</v>
       </c>
       <c r="D224" s="1">
-        <f>A224*E224</f>
+        <f t="shared" si="7"/>
         <v>54</v>
       </c>
       <c r="E224">
@@ -6089,11 +6089,11 @@
         <v>46</v>
       </c>
       <c r="C225" s="2">
-        <f>A225*E225*E225</f>
+        <f t="shared" si="6"/>
         <v>54</v>
       </c>
       <c r="D225" s="2">
-        <f>A225*E225</f>
+        <f t="shared" si="7"/>
         <v>54</v>
       </c>
       <c r="E225">
@@ -6111,11 +6111,11 @@
         <v>202</v>
       </c>
       <c r="C226" s="1">
-        <f>A226*E226*E226</f>
+        <f t="shared" si="6"/>
         <v>208</v>
       </c>
       <c r="D226" s="1">
-        <f>A226*E226</f>
+        <f t="shared" si="7"/>
         <v>52</v>
       </c>
       <c r="E226">
@@ -6133,11 +6133,11 @@
         <v>47</v>
       </c>
       <c r="C227" s="2">
-        <f>A227*E227*E227</f>
+        <f t="shared" si="6"/>
         <v>49</v>
       </c>
       <c r="D227" s="2">
-        <f>A227*E227</f>
+        <f t="shared" si="7"/>
         <v>49</v>
       </c>
       <c r="E227">
@@ -6155,11 +6155,11 @@
         <v>136</v>
       </c>
       <c r="C228" s="1">
-        <f>A228*E228*E228</f>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="D228" s="1">
-        <f>A228*E228</f>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="E228">
@@ -6177,11 +6177,11 @@
         <v>63</v>
       </c>
       <c r="C229" s="2">
-        <f>A229*E229*E229</f>
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
       <c r="D229" s="2">
-        <f>A229*E229</f>
+        <f t="shared" si="7"/>
         <v>45</v>
       </c>
       <c r="E229">
@@ -6199,11 +6199,11 @@
         <v>65</v>
       </c>
       <c r="C230" s="2">
-        <f>A230*E230*E230</f>
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
       <c r="D230" s="2">
-        <f>A230*E230</f>
+        <f t="shared" si="7"/>
         <v>45</v>
       </c>
       <c r="E230">
@@ -6221,11 +6221,11 @@
         <v>77</v>
       </c>
       <c r="C231" s="1">
-        <f>A231*E231*E231</f>
+        <f t="shared" si="6"/>
         <v>44</v>
       </c>
       <c r="D231" s="1">
-        <f>A231*E231</f>
+        <f t="shared" si="7"/>
         <v>44</v>
       </c>
       <c r="E231">
@@ -6243,11 +6243,11 @@
         <v>107</v>
       </c>
       <c r="C232" s="1">
-        <f>A232*E232*E232</f>
+        <f t="shared" si="6"/>
         <v>84</v>
       </c>
       <c r="D232" s="1">
-        <f>A232*E232</f>
+        <f t="shared" si="7"/>
         <v>42</v>
       </c>
       <c r="E232">
@@ -6265,11 +6265,11 @@
         <v>57</v>
       </c>
       <c r="C233" s="2">
-        <f>A233*E233*E233</f>
+        <f t="shared" si="6"/>
         <v>42</v>
       </c>
       <c r="D233" s="2">
-        <f>A233*E233</f>
+        <f t="shared" si="7"/>
         <v>42</v>
       </c>
       <c r="E233">
@@ -6287,11 +6287,11 @@
         <v>106</v>
       </c>
       <c r="C234" s="1">
-        <f>A234*E234*E234</f>
+        <f t="shared" si="6"/>
         <v>80</v>
       </c>
       <c r="D234" s="1">
-        <f>A234*E234</f>
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="E234">
@@ -6309,11 +6309,11 @@
         <v>78</v>
       </c>
       <c r="C235" s="1">
-        <f>A235*E235*E235</f>
+        <f t="shared" si="6"/>
         <v>39</v>
       </c>
       <c r="D235" s="1">
-        <f>A235*E235</f>
+        <f t="shared" si="7"/>
         <v>39</v>
       </c>
       <c r="E235">
@@ -6331,11 +6331,11 @@
         <v>241</v>
       </c>
       <c r="C236" s="1">
-        <f>A236*E236*E236</f>
+        <f t="shared" si="6"/>
         <v>76</v>
       </c>
       <c r="D236" s="1">
-        <f>A236*E236</f>
+        <f t="shared" si="7"/>
         <v>38</v>
       </c>
       <c r="E236">
@@ -6353,11 +6353,11 @@
         <v>54</v>
       </c>
       <c r="C237" s="2">
-        <f>A237*E237*E237</f>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="D237" s="2">
-        <f>A237*E237</f>
+        <f t="shared" si="7"/>
         <v>37</v>
       </c>
       <c r="E237">
@@ -6375,11 +6375,11 @@
         <v>64</v>
       </c>
       <c r="C238" s="2">
-        <f>A238*E238*E238</f>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="D238" s="2">
-        <f>A238*E238</f>
+        <f t="shared" si="7"/>
         <v>37</v>
       </c>
       <c r="E238">
@@ -6397,11 +6397,11 @@
         <v>66</v>
       </c>
       <c r="C239" s="2">
-        <f>A239*E239*E239</f>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="D239" s="2">
-        <f>A239*E239</f>
+        <f t="shared" si="7"/>
         <v>37</v>
       </c>
       <c r="E239">
@@ -6419,11 +6419,11 @@
         <v>100</v>
       </c>
       <c r="C240" s="2">
-        <f>A240*E240*E240</f>
+        <f t="shared" si="6"/>
         <v>72</v>
       </c>
       <c r="D240" s="2">
-        <f>A240*E240</f>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="E240">
@@ -6441,11 +6441,11 @@
         <v>55</v>
       </c>
       <c r="C241" s="2">
-        <f>A241*E241*E241</f>
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
       <c r="D241" s="2">
-        <f>A241*E241</f>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="E241">
@@ -6463,11 +6463,11 @@
         <v>56</v>
       </c>
       <c r="C242" s="2">
-        <f>A242*E242*E242</f>
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
       <c r="D242" s="2">
-        <f>A242*E242</f>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="E242">
@@ -6485,11 +6485,11 @@
         <v>137</v>
       </c>
       <c r="C243" s="1">
-        <f>A243*E243*E243</f>
+        <f t="shared" si="6"/>
         <v>35</v>
       </c>
       <c r="D243" s="1">
-        <f>A243*E243</f>
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
       <c r="E243">
@@ -6507,11 +6507,11 @@
         <v>59</v>
       </c>
       <c r="C244" s="2">
-        <f>A244*E244*E244</f>
+        <f t="shared" si="6"/>
         <v>34</v>
       </c>
       <c r="D244" s="2">
-        <f>A244*E244</f>
+        <f t="shared" si="7"/>
         <v>34</v>
       </c>
       <c r="E244">
@@ -6529,11 +6529,11 @@
         <v>62</v>
       </c>
       <c r="C245" s="2">
-        <f>A245*E245*E245</f>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="D245" s="2">
-        <f>A245*E245</f>
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
       <c r="E245">
@@ -6551,11 +6551,11 @@
         <v>61</v>
       </c>
       <c r="C246" s="2">
-        <f>A246*E246*E246</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="D246" s="2">
-        <f>A246*E246</f>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="E246">
@@ -6573,11 +6573,11 @@
         <v>5</v>
       </c>
       <c r="C247" s="1">
-        <f>A247*E247*E247</f>
+        <f t="shared" si="6"/>
         <v>29</v>
       </c>
       <c r="D247" s="1">
-        <f>A247*E247</f>
+        <f t="shared" si="7"/>
         <v>29</v>
       </c>
       <c r="E247">
@@ -6595,11 +6595,11 @@
         <v>201</v>
       </c>
       <c r="C248" s="1">
-        <f>A248*E248*E248</f>
+        <f t="shared" si="6"/>
         <v>112</v>
       </c>
       <c r="D248" s="1">
-        <f>A248*E248</f>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="E248">
@@ -6617,11 +6617,11 @@
         <v>249</v>
       </c>
       <c r="C249" s="1">
-        <f>A249*E249*E249</f>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="D249" s="1">
-        <f>A249*E249</f>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="E249">
@@ -6639,11 +6639,11 @@
         <v>60</v>
       </c>
       <c r="C250" s="2">
-        <f>A250*E250*E250</f>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="D250" s="2">
-        <f>A250*E250</f>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="E250">
@@ -6661,11 +6661,11 @@
         <v>109</v>
       </c>
       <c r="C251" s="1">
-        <f>A251*E251*E251</f>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="D251" s="1">
-        <f>A251*E251</f>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
       <c r="E251">
@@ -6683,11 +6683,11 @@
         <v>108</v>
       </c>
       <c r="C252" s="1">
-        <f>A252*E252*E252</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="D252" s="1">
-        <f>A252*E252</f>
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="E252">
@@ -6705,11 +6705,11 @@
         <v>110</v>
       </c>
       <c r="C253" s="1">
-        <f>A253*E253*E253</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="D253" s="1">
-        <f>A253*E253</f>
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
       <c r="E253">
@@ -6727,11 +6727,11 @@
         <v>111</v>
       </c>
       <c r="C254" s="1">
-        <f>A254*E254*E254</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="D254" s="1">
-        <f>A254*E254</f>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="E254">
@@ -6749,11 +6749,11 @@
         <v>58</v>
       </c>
       <c r="C255" s="2">
-        <f>A255*E255*E255</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="D255" s="2">
-        <f>A255*E255</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="E255">
@@ -6771,11 +6771,11 @@
         <v>0</v>
       </c>
       <c r="C256" s="2">
-        <f>A256*E256*E256</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D256" s="2">
-        <f>A256*E256</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E256">
@@ -6793,11 +6793,11 @@
         <v>89</v>
       </c>
       <c r="C257" s="1">
-        <f>A257*E257*E257</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D257" s="1">
-        <f>A257*E257</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E257">

</xml_diff>

<commit_message>
Added Small Appartments 2
</commit_message>
<xml_diff>
--- a/building_stats.xlsx
+++ b/building_stats.xlsx
@@ -1150,7 +1150,7 @@
   <dimension ref="A1:F257"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2587,14 +2587,14 @@
       <c r="A66">
         <v>1165</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="2">
         <v>141</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="2">
         <f t="shared" ref="C66:C129" si="2">A66*E66*E66</f>
         <v>4660</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66" s="2">
         <f t="shared" ref="D66:D129" si="3">A66*E66</f>
         <v>2330</v>
       </c>

</xml_diff>

<commit_message>
Added Small Appartments 3
Added Small Appartments 3 building
</commit_message>
<xml_diff>
--- a/building_stats.xlsx
+++ b/building_stats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="135" windowWidth="9540" windowHeight="10260"/>
@@ -1150,7 +1150,7 @@
   <dimension ref="A1:F257"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+      <selection activeCell="B70" sqref="B70:D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2675,14 +2675,14 @@
       <c r="A70">
         <v>1120</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="2">
         <v>142</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C70" s="2">
         <f t="shared" si="2"/>
         <v>4480</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D70" s="2">
         <f t="shared" si="3"/>
         <v>2240</v>
       </c>

</xml_diff>

<commit_message>
Added Hydro 2 (building 199)
</commit_message>
<xml_diff>
--- a/building_stats.xlsx
+++ b/building_stats.xlsx
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="B219" sqref="B219:D219"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76:D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2807,14 +2807,14 @@
       <c r="A76">
         <v>1942</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76" s="2">
         <v>199</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="2">
         <f t="shared" si="2"/>
         <v>1942</v>
       </c>
-      <c r="D76" s="1">
+      <c r="D76" s="2">
         <f t="shared" si="3"/>
         <v>1942</v>
       </c>

</xml_diff>

<commit_message>
Added Hydro 1 (building 198)
</commit_message>
<xml_diff>
--- a/building_stats.xlsx
+++ b/building_stats.xlsx
@@ -1150,7 +1150,7 @@
   <dimension ref="A1:F257"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76:D76"/>
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2851,14 +2851,14 @@
       <c r="A78">
         <v>1821</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78" s="2">
         <v>198</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="2">
         <f t="shared" si="2"/>
         <v>1821</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D78" s="2">
         <f t="shared" si="3"/>
         <v>1821</v>
       </c>

</xml_diff>